<commit_message>
Add extra validations, logs and optimization
</commit_message>
<xml_diff>
--- a/out/merged.xlsx
+++ b/out/merged.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>cliente</t>
+          <t>client</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>importe</t>
+          <t>value</t>
         </is>
       </c>
     </row>

</xml_diff>